<commit_message>
updated list of metrics
</commit_message>
<xml_diff>
--- a/list_of_metrics.xlsx
+++ b/list_of_metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\_coding\lidRmetrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D424FF4B-7A53-4AEC-BCF8-7EC74778EA18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9668C77E-8996-43F8-85F4-3A46AF5491C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -236,9 +236,6 @@
     <t>McGaughey, R.J., 2021. FUSION/LDV: Software for LIDAR Data Analysis and Visualization. http://forsys.cfr.washington.edu/software/fusion/FUSION_manual.pdf</t>
   </si>
   <si>
-    <t>kde_peaks_count, kde_peaks_elev, kde_peaks_value</t>
-  </si>
-  <si>
     <t>metrics_echo</t>
   </si>
   <si>
@@ -263,9 +260,6 @@
     <t>filled ratio; FRall - a ratio between the number of filled voxels and all voxels located in the maximum extent of the point cloud. In case of  FRcanopy empty voxels above the canopy are excluded in the calculations</t>
   </si>
   <si>
-    <t>Kernel density estimation applied to the distribution of point cloud elevation (Z). KDE allows to create a probability density function (using a Guassian kernel). The density function is then used to detect peaks (function maxima). Based on similar metric available in Fusion (see references), modified.</t>
-  </si>
-  <si>
     <t>metrics_texture</t>
   </si>
   <si>
@@ -276,6 +270,12 @@
   </si>
   <si>
     <t>requires the {ForestTools} package. ForestTools::glcm_img() function is used to calculate the GLCM statistics (see package manual for details)</t>
+  </si>
+  <si>
+    <t>kde_peaks_count, kde_peak1_elev,  kde_peak2_elev, …, kde_peak1_value, kde_peak2_value, …, kde_peak1_diff, kde_peak2_diff, …</t>
+  </si>
+  <si>
+    <t>Based on similar metric available in Fusion (see references), with significant differences in the list of output statistics as well as the default bandwidth used when estimating kernel density.</t>
   </si>
 </sst>
 </file>
@@ -655,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +849,7 @@
         <v>45</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s">
         <v>41</v>
@@ -893,10 +893,10 @@
     </row>
     <row r="20" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
         <v>52</v>
@@ -907,41 +907,41 @@
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" t="s">
         <v>59</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="270" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated table in readme
</commit_message>
<xml_diff>
--- a/list_of_metrics.xlsx
+++ b/list_of_metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\_coding\lidRmetrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8771790F-797D-405A-9466-40FF8AEEF50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94353F1E-A581-4CA5-BEDA-FE2D62A0B901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23130" yWindow="0" windowWidth="21480" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24435" yWindow="705" windowWidth="23010" windowHeight="14970" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -288,9 +288,6 @@
     <t>Proportion of returns by echo types (First, Intermediate, Last; and Single, Multiple)</t>
   </si>
   <si>
-    <t>ratio_first_last, ratio_first_intermediate, ratio_multiple_single</t>
-  </si>
-  <si>
     <t>Ratios of return counts</t>
   </si>
   <si>
@@ -308,13 +305,16 @@
   </si>
   <si>
     <t>n_return_1, n_return_2, …, n_return_*</t>
+  </si>
+  <si>
+    <t>ratio_last_first, ratio_intermediate_first, ratio_multiple_single</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -344,12 +344,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Lucida Console"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -371,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -385,9 +379,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -773,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -920,7 +911,7 @@
     </row>
     <row r="12" spans="1:4" ht="31.5">
       <c r="A12" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>32</v>
@@ -929,7 +920,7 @@
         <v>33</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="60">
@@ -967,24 +958,24 @@
     </row>
     <row r="16" spans="1:4" ht="45">
       <c r="A16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="C16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="6" t="s">
-        <v>76</v>
+    <row r="17" spans="1:4" ht="36" customHeight="1">
+      <c r="A17" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:4">

</xml_diff>

<commit_message>
added shortcut function to each metric. fix #14
</commit_message>
<xml_diff>
--- a/list_of_metrics.xlsx
+++ b/list_of_metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\_coding\lidRmetrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94353F1E-A581-4CA5-BEDA-FE2D62A0B901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353C2C04-4A35-47E6-AB17-B7F4564F1CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24435" yWindow="705" windowWidth="23010" windowHeight="14970" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15" yWindow="900" windowWidth="23010" windowHeight="14970" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -764,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>

</xml_diff>